<commit_message>
atualização da tabela de tempo de execução + arquivos de ordenação
</commit_message>
<xml_diff>
--- a/bucket_sort.xlsx
+++ b/bucket_sort.xlsx
@@ -5,45 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Documents\mestrado\paa\BucketSort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Documents\mestrado\paa\BucketSort\Bucket-Sort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BB11AC-37EC-4C95-B3EA-2636931B2C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D3D41F-1B70-4E4C-8109-099AB854C552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{639CA21C-F7A9-416D-9100-AB0319DBCEC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{639CA21C-F7A9-416D-9100-AB0319DBCEC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="100%" sheetId="1" r:id="rId1"/>
+    <sheet name="50%" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Planilha1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Planilha1!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Planilha1!$C$2:$C$10</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Planilha1!$D$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Planilha1!$D$2:$D$10</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Planilha1!$E$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Planilha1!$E$2:$E$10</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Planilha1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Planilha1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Planilha1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Planilha1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Planilha1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Planilha1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Planilha1!$A$2:$A$10</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>IS</t>
   </si>
@@ -87,7 +59,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -126,14 +98,34 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -141,23 +133,29 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -266,7 +264,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$1</c:f>
+              <c:f>'100%'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +314,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -352,7 +350,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$2:$B$10</c:f>
+              <c:f>'100%'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -397,7 +395,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$C$1</c:f>
+              <c:f>'100%'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -447,7 +445,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -483,7 +481,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$2:$C$10</c:f>
+              <c:f>'100%'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -528,7 +526,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$D$1</c:f>
+              <c:f>'100%'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -578,7 +576,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -614,7 +612,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$D$2:$D$10</c:f>
+              <c:f>'100%'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -659,7 +657,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$E$1</c:f>
+              <c:f>'100%'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -709,7 +707,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -745,7 +743,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$E$2:$E$10</c:f>
+              <c:f>'100%'!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -925,7 +923,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -958,7 +956,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1163,7 +1161,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$1</c:f>
+              <c:f>'100%'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1234,7 +1232,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1270,7 +1268,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$2:$B$10</c:f>
+              <c:f>'100%'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1316,7 +1314,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$C$1</c:f>
+              <c:f>'100%'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1387,7 +1385,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1423,7 +1421,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$2:$C$10</c:f>
+              <c:f>'100%'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1469,7 +1467,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$D$1</c:f>
+              <c:f>'100%'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1540,7 +1538,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1576,7 +1574,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$D$2:$D$10</c:f>
+              <c:f>'100%'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1622,7 +1620,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$E$1</c:f>
+              <c:f>'100%'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1693,7 +1691,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'100%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1729,7 +1727,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$E$2:$E$10</c:f>
+              <c:f>'100%'!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2060,35 +2058,35 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr kumimoji="0" lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:uLnTx/>
-                <a:uFillTx/>
-                <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-              </a:rPr>
-              <a:t>InsertionSort</a:t>
+              <a:rPr lang="pt-BR"/>
+              <a:t>BucketSort para metade</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> dos baldes</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>:</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2106,13 +2104,917 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.5070000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7429999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.023999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1046.0529999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10239.281999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20994.411</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68863.057000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>114514.871</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D9AD-47BB-A4BB-DCF8BADA38F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4949999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1065.145</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10448.295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20499.645</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75067.724000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>117547.60400000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D9AD-47BB-A4BB-DCF8BADA38F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.99599999999999989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1128.836</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10592.081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20777.488999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>67679.501000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>151321.45800000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D9AD-47BB-A4BB-DCF8BADA38F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.774</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9980000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.129000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1005.1349999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10512.014000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19929.259999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69132.615000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>148169.541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D9AD-47BB-A4BB-DCF8BADA38F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1143597327"/>
+        <c:axId val="1272840736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1143597327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Tamanho do vetor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1272840736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1272840736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Tempo (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1143597327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -2126,14 +3028,14 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$1</c:f>
+              <c:f>'50%'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2145,7 +3047,7 @@
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2164,21 +3066,21 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent6">
+                    <a:schemeClr val="accent1">
                       <a:satMod val="103000"/>
                       <a:lumMod val="102000"/>
                       <a:tint val="94000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="50000">
-                    <a:schemeClr val="accent6">
+                    <a:schemeClr val="accent1">
                       <a:satMod val="110000"/>
                       <a:lumMod val="100000"/>
                       <a:shade val="100000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
+                    <a:schemeClr val="accent1">
                       <a:lumMod val="99000"/>
                       <a:satMod val="120000"/>
                       <a:shade val="78000"/>
@@ -2189,7 +3091,7 @@
               </a:gradFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -2202,67 +3104,9 @@
               </a:effectLst>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$10</c:f>
+              <c:f>'50%'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2298,36 +3142,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$2:$B$10</c:f>
+              <c:f>'50%'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.5070000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99778175354003906</c:v>
+                  <c:v>1.7429999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.90727615356445</c:v>
+                  <c:v>2.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.043716430663999</c:v>
+                  <c:v>40.023999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1417.9790019989</c:v>
+                  <c:v>1046.0529999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10929.640531539899</c:v>
+                  <c:v>10239.281999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19385.973453521699</c:v>
+                  <c:v>20994.411</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79198.0500221252</c:v>
+                  <c:v>68863.057000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>218812.31689453099</c:v>
+                  <c:v>114514.871</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,14 +3179,472 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8AA5-4B68-A8D6-0E58BA410D0B}"/>
+              <c16:uniqueId val="{00000000-DD2D-42ED-A280-BB77CBCE3DC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4949999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1065.145</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10448.295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20499.645</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75067.724000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>117547.60400000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD2D-42ED-A280-BB77CBCE3DC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.99599999999999989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1128.836</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10592.081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20777.488999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>67679.501000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>151321.45800000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DD2D-42ED-A280-BB77CBCE3DC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50%'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'50%'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50%'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.774</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9980000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.129000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1005.1349999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10512.014000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19929.259999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69132.615000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>148169.541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DD2D-42ED-A280-BB77CBCE3DC7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2350,27 +3652,56 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1357550095"/>
-        <c:axId val="1274377904"/>
+        <c:axId val="260442112"/>
+        <c:axId val="1336361423"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1357550095"/>
+        <c:axId val="260442112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2384,9 +3715,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2397,7 +3727,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1274377904"/>
+        <c:crossAx val="1336361423"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2405,7 +3735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1274377904"/>
+        <c:axId val="1336361423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,9 +3745,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2425,6 +3755,35 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2443,9 +3802,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2456,7 +3814,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1357550095"/>
+        <c:crossAx val="260442112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2468,8 +3826,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2480,17 +3868,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -2593,10 +3992,53 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -3622,35 +5064,33 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3658,37 +5098,44 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3707,14 +5154,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -3803,252 +5242,251 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:seriesLine>
   <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4072,9 +5510,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4084,7 +5521,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4092,9 +5529,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4105,11 +5542,506 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4117,7 +6049,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -4127,16 +6059,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>100011</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47630</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>404811</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4197,29 +6129,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>78921</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>117700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>404811</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>326571</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>179613</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6868FE40-2AC4-8F67-3116-A9C809CC9E82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0F812A4-06FA-4995-A9FA-48EC298B8595}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4227,7 +6166,45 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>184162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4DD9D6-23B1-4BD0-8393-93DC2046C154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4237,14 +6214,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36B08ED9-E849-4F26-817F-CE81F96B6D58}" name="Tabela1" displayName="Tabela1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36B08ED9-E849-4F26-817F-CE81F96B6D58}" name="Tabela1" displayName="Tabela1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E10" xr:uid="{36B08ED9-E849-4F26-817F-CE81F96B6D58}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{01F3B5CB-057E-406D-8088-8A84E15C81E6}" name="Size" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{1F44DD9C-B16C-4EA6-A872-3B6DA18CCF01}" name="IS" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A3280B14-5850-4538-8A4C-973AE7B394A0}" name="QS" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{6B36471B-F289-4F72-8FCA-27E0D7423E05}" name="MS" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{FD79200C-D9D4-4B45-8132-53E034063A1A}" name="HS" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{01F3B5CB-057E-406D-8088-8A84E15C81E6}" name="Size" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{1F44DD9C-B16C-4EA6-A872-3B6DA18CCF01}" name="IS" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A3280B14-5850-4538-8A4C-973AE7B394A0}" name="QS" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{6B36471B-F289-4F72-8FCA-27E0D7423E05}" name="MS" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{FD79200C-D9D4-4B45-8132-53E034063A1A}" name="HS" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3635C52A-D5CA-4584-B483-48CF98BB99F9}" name="Tabela13" displayName="Tabela13" ref="A1:E10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E10" xr:uid="{36B08ED9-E849-4F26-817F-CE81F96B6D58}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2048F242-657C-41B7-AE47-2E14A23AA537}" name="Size" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{7B58AFF3-BBB8-4074-BE84-043BE10A5D10}" name="IS" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F61C8980-8DEF-4C67-8E48-0AD2697BC06D}" name="QS" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{DB0AAAFA-66A0-4C22-9830-E6861CA167C8}" name="MS" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3A38B6FF-4A41-4458-A82F-668AFFCEC5C9}" name="HS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4569,8 +6560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF383E5-8B21-4558-A6E4-4F99F8AD8303}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4801,23 +6792,290 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Planilha1!C:C</xm:f>
+              <xm:f>'100%'!C:C</xm:f>
               <xm:sqref>R8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Planilha1!C:C</xm:f>
+              <xm:f>'100%'!C:C</xm:f>
               <xm:sqref>R9</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Planilha1!C:C</xm:f>
+              <xm:f>'100%'!C:C</xm:f>
               <xm:sqref>R10</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Planilha1!C:C</xm:f>
+              <xm:f>'100%'!C:C</xm:f>
               <xm:sqref>R11</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Planilha1!C:C</xm:f>
+              <xm:f>'100%'!C:C</xm:f>
+              <xm:sqref>R12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E342B1F3-AF1F-46F0-BC70-D02735944337}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3">
+        <f>1000*0.001507</f>
+        <v>1.5070000000000001</v>
+      </c>
+      <c r="C2" s="3">
+        <f>1000*0.001045</f>
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="D2" s="3">
+        <f>1000*0.000996</f>
+        <v>0.99599999999999989</v>
+      </c>
+      <c r="E2" s="3">
+        <f>1000*0.001774</f>
+        <v>1.774</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>500</v>
+      </c>
+      <c r="B3" s="3">
+        <f>1000*0.001743</f>
+        <v>1.7429999999999999</v>
+      </c>
+      <c r="C3" s="3">
+        <f>1000*0.002267</f>
+        <v>2.2669999999999999</v>
+      </c>
+      <c r="D3" s="3">
+        <f>1000*0.001484</f>
+        <v>1.484</v>
+      </c>
+      <c r="E3" s="3">
+        <f>0.00174*1000</f>
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B4" s="3">
+        <f>1000*0.00273</f>
+        <v>2.73</v>
+      </c>
+      <c r="C4" s="3">
+        <f>1000*0.003495</f>
+        <v>3.4949999999999997</v>
+      </c>
+      <c r="D4" s="3">
+        <f>1000*0.001584</f>
+        <v>1.5839999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <f>1000*0.001998</f>
+        <v>1.9980000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="B5" s="3">
+        <f>1000*0.040024</f>
+        <v>40.023999999999994</v>
+      </c>
+      <c r="C5" s="3">
+        <f>1000*0.03125</f>
+        <v>31.25</v>
+      </c>
+      <c r="D5" s="3">
+        <f>1000*0.02544</f>
+        <v>25.44</v>
+      </c>
+      <c r="E5" s="3">
+        <f>1000*0.028129</f>
+        <v>28.129000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>30000</v>
+      </c>
+      <c r="B6" s="3">
+        <f>1000*1.046053</f>
+        <v>1046.0529999999999</v>
+      </c>
+      <c r="C6" s="3">
+        <f>1000*1.065145</f>
+        <v>1065.145</v>
+      </c>
+      <c r="D6" s="3">
+        <f>1000*1.128836</f>
+        <v>1128.836</v>
+      </c>
+      <c r="E6" s="3">
+        <f>1000*1.005135</f>
+        <v>1005.1349999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>80000</v>
+      </c>
+      <c r="B7" s="3">
+        <f>1000*10.239282</f>
+        <v>10239.281999999999</v>
+      </c>
+      <c r="C7" s="3">
+        <f>1000*10.448295</f>
+        <v>10448.295</v>
+      </c>
+      <c r="D7" s="3">
+        <f>1000*10.592081</f>
+        <v>10592.081</v>
+      </c>
+      <c r="E7" s="3">
+        <f>1000*10.512014</f>
+        <v>10512.014000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B8" s="3">
+        <f>1000*20.994411</f>
+        <v>20994.411</v>
+      </c>
+      <c r="C8" s="3">
+        <f>1000*20.499645</f>
+        <v>20499.645</v>
+      </c>
+      <c r="D8" s="3">
+        <f>1000*20.777489</f>
+        <v>20777.488999999998</v>
+      </c>
+      <c r="E8" s="3">
+        <f>1000*19.92926</f>
+        <v>19929.259999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>150000</v>
+      </c>
+      <c r="B9" s="3">
+        <f>1000*68.863057</f>
+        <v>68863.057000000001</v>
+      </c>
+      <c r="C9" s="3">
+        <f>1000*75.067724</f>
+        <v>75067.724000000002</v>
+      </c>
+      <c r="D9" s="3">
+        <f>1000*67.679501</f>
+        <v>67679.501000000004</v>
+      </c>
+      <c r="E9" s="3">
+        <f>1000*69.132615</f>
+        <v>69132.615000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>200000</v>
+      </c>
+      <c r="B10" s="3">
+        <f>114.514871  *1000</f>
+        <v>114514.871</v>
+      </c>
+      <c r="C10" s="3">
+        <f>1000*117.547604</f>
+        <v>117547.60400000001</v>
+      </c>
+      <c r="D10" s="3">
+        <f>1000*151.321458</f>
+        <v>151321.45800000001</v>
+      </c>
+      <c r="E10" s="3">
+        <f>1000*148.169541</f>
+        <v>148169.541</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{32933C85-FE9B-4C09-8AE0-1CCDDFE1C44F}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'50%'!C:C</xm:f>
+              <xm:sqref>R8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'50%'!C:C</xm:f>
+              <xm:sqref>R9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'50%'!C:C</xm:f>
+              <xm:sqref>R10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'50%'!C:C</xm:f>
+              <xm:sqref>R11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'50%'!C:C</xm:f>
               <xm:sqref>R12</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>

</xml_diff>